<commit_message>
some changes in Skills Section
</commit_message>
<xml_diff>
--- a/Documents/Tableau de synthese Epreuve E4.xlsx
+++ b/Documents/Tableau de synthese Epreuve E4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\OneDrive\Bureau\DEV.EXE\DEV SIO1\PORTFOLIO\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\OneDrive\Bureau\DEV.EXE\DEV SIO1\Portfolio - Joshua Thebaudin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4408C12B-0B9D-4744-8905-FD7CC8F682E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0D49D4-F07F-4055-8F51-AD5AA8DD1CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>Réalisations en milieu professionnel en cours de seconde année</t>
-  </si>
-  <si>
-    <t>Adresse URL du portfolio :</t>
   </si>
   <si>
     <t>NOM et prénom : Thebaudin Joshua</t>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t xml:space="preserve">Déploiement de l'application en interne </t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://josthb.github.io/Portfolio-Joshua_Thebaudin/</t>
   </si>
 </sst>
 </file>
@@ -751,15 +751,39 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -791,30 +815,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1162,7 +1162,7 @@
   <dimension ref="A1:AQ81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A5" sqref="A5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1175,56 +1175,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="29"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:43" ht="40.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="47" t="s">
+      <c r="A3" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="48"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="35"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="46"/>
+      <c r="A4" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1232,26 +1232,26 @@
         <v>15</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="40"/>
+      <c r="A5" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="48"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="44" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1274,8 +1274,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1331,16 +1331,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="40"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1379,7 +1379,7 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="16"/>
@@ -1426,7 +1426,7 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="17"/>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="17"/>
@@ -1834,16 +1834,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="43"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1882,7 +1882,7 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="17"/>
@@ -1929,7 +1929,7 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="17"/>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="17"/>
@@ -2023,7 +2023,7 @@
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="17"/>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="17"/>
@@ -2206,16 +2206,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="35"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="43"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2660,11 +2660,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2672,6 +2667,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2682,18 +2682,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2811,18 +2811,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F6BD27-A3F1-4936-A454-42BABB06C263}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7A83CDF-503E-4E47-92C2-3FA62E9FFE8B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7A83CDF-503E-4E47-92C2-3FA62E9FFE8B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F6BD27-A3F1-4936-A454-42BABB06C263}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Maj du Portfolio | ajout sdossier complémentaire AMAPBIO
</commit_message>
<xml_diff>
--- a/Documents/Tableau de synthese Epreuve E4.xlsx
+++ b/Documents/Tableau de synthese Epreuve E4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\OneDrive\Bureau\DEV.EXE\DEV SIO1\Portfolio - Joshua Thebaudin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54D49DF-8F51-4B2A-93FF-077AEB28AA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028A10B7-A6CB-4F7C-A081-FEA60728C9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -150,9 +150,6 @@
     </r>
   </si>
   <si>
-    <t>STAGE 1ère Année SILENTSYS (16 Mai - 17 Juin 2022)</t>
-  </si>
-  <si>
     <t>PPE 1  (1er semestre de 1ére année) : Utilisation des CMS</t>
   </si>
   <si>
@@ -187,6 +184,21 @@
   </si>
   <si>
     <t>16/05 - 17/06</t>
+  </si>
+  <si>
+    <t>STAGE 2ème MINDFUL-HOUSE (3 janvier - 10 février 2023)</t>
+  </si>
+  <si>
+    <t>STAGE 1ère Année SILENTSYS (16 mai - 17 juin 2022)</t>
+  </si>
+  <si>
+    <t>03/01 - 10/02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Documentation sur le langage JS et le framework React ainsi que ses librairies</t>
+  </si>
+  <si>
+    <t>Documentation sur GIT</t>
   </si>
 </sst>
 </file>
@@ -196,7 +208,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -266,6 +278,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -678,7 +696,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -755,15 +773,45 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -797,34 +845,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1171,8 +1192,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1211,30 +1232,30 @@
       <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="46" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="47"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="36"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1246,22 +1267,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
+      <c r="A5" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="49"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="45" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1284,8 +1305,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1341,16 +1362,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="41"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1389,12 +1410,12 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="48"/>
+        <v>26</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="26"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
       <c r="F9" s="21"/>
@@ -1438,10 +1459,10 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
@@ -1487,10 +1508,10 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
@@ -1850,16 +1871,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="44"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1898,10 +1919,10 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
@@ -1947,7 +1968,7 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="16"/>
@@ -1994,7 +2015,7 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="21"/>
@@ -2041,7 +2062,7 @@
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="16"/>
@@ -2088,7 +2109,7 @@
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="16"/>
@@ -2224,16 +2245,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="34"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="44"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2271,8 +2292,12 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="10"/>
+      <c r="A28" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -2316,12 +2341,14 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
+      <c r="A29" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="B29" s="10"/>
       <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
+      <c r="D29" s="21"/>
       <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
+      <c r="F29" s="21"/>
       <c r="G29" s="16"/>
       <c r="H29" s="17"/>
       <c r="I29"/>
@@ -2361,14 +2388,16 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
+      <c r="A30" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="B30" s="10"/>
-      <c r="C30" s="16"/>
+      <c r="C30" s="21"/>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
-      <c r="H30" s="17"/>
+      <c r="H30" s="22"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2406,14 +2435,16 @@
       <c r="AQ30"/>
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+      <c r="A31" s="50" t="s">
+        <v>42</v>
+      </c>
       <c r="B31" s="10"/>
-      <c r="C31" s="16"/>
+      <c r="C31" s="21"/>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
+      <c r="F31" s="23"/>
       <c r="G31" s="16"/>
-      <c r="H31" s="17"/>
+      <c r="H31" s="22"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2451,12 +2482,14 @@
       <c r="AQ31"/>
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
+      <c r="A32" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="B32" s="10"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="16"/>
       <c r="H32" s="17"/>
       <c r="I32"/>
@@ -2678,11 +2711,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2690,6 +2718,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2700,18 +2733,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2829,6 +2862,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7A83CDF-503E-4E47-92C2-3FA62E9FFE8B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F6BD27-A3F1-4936-A454-42BABB06C263}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -2839,14 +2880,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7A83CDF-503E-4E47-92C2-3FA62E9FFE8B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Maj du Portfolio | ajout projet C# + correction pb ui
</commit_message>
<xml_diff>
--- a/Documents/Tableau de synthese Epreuve E4.xlsx
+++ b/Documents/Tableau de synthese Epreuve E4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\OneDrive\Bureau\DEV.EXE\DEV SIO1\Portfolio - Joshua Thebaudin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028A10B7-A6CB-4F7C-A081-FEA60728C9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A041C4-FDA9-4085-BBAA-E944159EED59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -96,12 +96,6 @@
     <t>Compétences mises en œuvre
 Réalisations professionnelles
 (intitulé et liste des documents et productions associés)</t>
-  </si>
-  <si>
-    <t>SESSION 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N° candidat : </t>
   </si>
   <si>
     <t>Période (sous la forme du JJ/MM/AA au JJ/MM/AA)</t>
@@ -183,22 +177,37 @@
     <t>09/22 - 12/22</t>
   </si>
   <si>
-    <t>16/05 - 17/06</t>
-  </si>
-  <si>
     <t>STAGE 2ème MINDFUL-HOUSE (3 janvier - 10 février 2023)</t>
   </si>
   <si>
     <t>STAGE 1ère Année SILENTSYS (16 mai - 17 juin 2022)</t>
   </si>
   <si>
-    <t>03/01 - 10/02</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Documentation sur le langage JS et le framework React ainsi que ses librairies</t>
   </si>
   <si>
     <t>Documentation sur GIT</t>
+  </si>
+  <si>
+    <t>PPE 4 (2ème semestre de 2ème année : Interface administrateur de contenu d'un site de commerce (C#)</t>
+  </si>
+  <si>
+    <t>01/23 - 04/23</t>
+  </si>
+  <si>
+    <t>SESSION 2023</t>
+  </si>
+  <si>
+    <t>N° candidat : 02243931005</t>
+  </si>
+  <si>
+    <t>16/05/2022 - 17/06/2022</t>
+  </si>
+  <si>
+    <t>03/01/2023 - 10/02/2023</t>
+  </si>
+  <si>
+    <t>Développement de l'application (ReactJS)</t>
   </si>
 </sst>
 </file>
@@ -779,6 +788,9 @@
     <xf numFmtId="17" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -844,9 +856,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1192,70 +1201,70 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="70.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" style="1" customWidth="1"/>
-    <col min="3" max="8" width="18.6640625" style="1" customWidth="1"/>
-    <col min="9" max="43" width="11.5546875" customWidth="1"/>
-    <col min="44" max="16384" width="10.77734375" style="1"/>
+    <col min="1" max="1" width="70.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
+    <col min="3" max="8" width="18.7109375" style="1" customWidth="1"/>
+    <col min="9" max="43" width="11.5703125" customWidth="1"/>
+    <col min="44" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:43" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="28"/>
-    </row>
-    <row r="2" spans="1:43" ht="40.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="29"/>
+    </row>
+    <row r="2" spans="1:43" ht="40.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-    </row>
-    <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="36"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:43" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="31"/>
+      <c r="H3" s="37"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
+    <row r="4" spans="1:43" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1263,27 +1272,27 @@
         <v>15</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="49"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="50"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="45" t="s">
-        <v>20</v>
+      <c r="B6" s="46" t="s">
+        <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>0</v>
@@ -1304,9 +1313,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
-      <c r="B7" s="46"/>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="325.14999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1361,17 +1370,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="42"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1408,12 +1417,12 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="26"/>
       <c r="D9" s="16"/>
@@ -1457,12 +1466,12 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
@@ -1506,12 +1515,12 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
@@ -1555,15 +1564,19 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="16"/>
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="21"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="17"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1600,7 +1613,7 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="10"/>
       <c r="C13" s="16"/>
@@ -1645,7 +1658,7 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="10"/>
       <c r="C14" s="16"/>
@@ -1690,7 +1703,7 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="10"/>
       <c r="C15" s="16"/>
@@ -1735,7 +1748,7 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="10"/>
       <c r="C16" s="16"/>
@@ -1780,7 +1793,7 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="10"/>
       <c r="C17" s="16"/>
@@ -1825,7 +1838,7 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="10"/>
       <c r="C18" s="16"/>
@@ -1870,17 +1883,17 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="44"/>
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="45"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1917,12 +1930,12 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
@@ -1966,9 +1979,9 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="16"/>
@@ -2013,9 +2026,9 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="21"/>
@@ -2060,9 +2073,9 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="16"/>
@@ -2107,9 +2120,9 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="16"/>
@@ -2154,7 +2167,7 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="10"/>
       <c r="C25" s="16"/>
@@ -2199,7 +2212,7 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="10"/>
       <c r="C26" s="16"/>
@@ -2244,17 +2257,17 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="44"/>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="45"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2291,12 +2304,12 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -2340,9 +2353,9 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="16"/>
@@ -2387,9 +2400,9 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="21"/>
@@ -2434,9 +2447,9 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="50" t="s">
-        <v>42</v>
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="28" t="s">
+        <v>38</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="21"/>
@@ -2481,9 +2494,9 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="16"/>
@@ -2528,7 +2541,7 @@
       <c r="AP32"/>
       <c r="AQ32"/>
     </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
       <c r="B33" s="10"/>
       <c r="C33" s="16"/>
@@ -2573,7 +2586,7 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="13"/>
       <c r="C34" s="18"/>
@@ -2618,7 +2631,7 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -2663,52 +2676,52 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A6:A7"/>

</xml_diff>